<commit_message>
all rating controllers done
</commit_message>
<xml_diff>
--- a/trash/progress.xlsx
+++ b/trash/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\merged_sajt\trash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC81178A-5BE1-4847-9C15-4EC247EAF934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982B3B64-EEA0-41A6-A7A0-63CE3A74C741}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" activeTab="2" xr2:uid="{012A0DE3-469E-4392-99CD-5887BA5AC192}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="181">
   <si>
     <t>Active_Password_Reset</t>
   </si>
@@ -445,24 +445,12 @@
     <t>arrayize</t>
   </si>
   <si>
-    <t>authorize</t>
-  </si>
-  <si>
     <t>check dependencies</t>
   </si>
   <si>
-    <t>prepare</t>
-  </si>
-  <si>
-    <t>create</t>
-  </si>
-  <si>
     <t>validate documents</t>
   </si>
   <si>
-    <t>save</t>
-  </si>
-  <si>
     <t>reply</t>
   </si>
   <si>
@@ -475,9 +463,6 @@
     <t>find</t>
   </si>
   <si>
-    <t>remove</t>
-  </si>
-  <si>
     <t>authorize find</t>
   </si>
   <si>
@@ -490,9 +475,6 @@
     <t>authorize update</t>
   </si>
   <si>
-    <t>prepare find</t>
-  </si>
-  <si>
     <t>authorize remove</t>
   </si>
   <si>
@@ -502,58 +484,94 @@
     <t>C,O,R,S</t>
   </si>
   <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>active_password_reset</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>entry_fee_payment</t>
+  </si>
+  <si>
+    <t>rating_picture</t>
+  </si>
+  <si>
+    <t>validate data</t>
+  </si>
+  <si>
+    <t>approve_dependent_mutations:</t>
+  </si>
+  <si>
+    <t>authorizer</t>
+  </si>
+  <si>
+    <t>other:</t>
+  </si>
+  <si>
+    <t>helpers:</t>
+  </si>
+  <si>
+    <t>rating_satisfies_sheet</t>
+  </si>
+  <si>
+    <t>rating_sheet_of_category_id</t>
+  </si>
+  <si>
+    <t>global authorizer mw</t>
+  </si>
+  <si>
+    <t>authorize create</t>
+  </si>
+  <si>
+    <t>save created documents</t>
+  </si>
+  <si>
+    <t>create locally</t>
+  </si>
+  <si>
+    <t>validate created documents</t>
+  </si>
+  <si>
+    <t>start session and transaction</t>
+  </si>
+  <si>
+    <t>validate new documents.</t>
+  </si>
+  <si>
+    <t>check dependencies.</t>
+  </si>
+  <si>
+    <t>commit transaction and end session.</t>
+  </si>
+  <si>
+    <t>check local dependencies + coll integrity</t>
+  </si>
+  <si>
+    <t>validate documents.</t>
+  </si>
+  <si>
+    <t>remove documents.</t>
+  </si>
+  <si>
+    <t>check local constraints and collection integrity</t>
+  </si>
+  <si>
+    <t>all validators</t>
+  </si>
+  <si>
     <t>update locally</t>
   </si>
   <si>
     <t>save updated documents</t>
   </si>
   <si>
-    <t>validate new documents</t>
-  </si>
-  <si>
-    <t>check collection integrity</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>active_password_reset</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>entry_fee_payment</t>
-  </si>
-  <si>
-    <t>rating_picture</t>
-  </si>
-  <si>
-    <t>validate data</t>
-  </si>
-  <si>
-    <t>approve_dependent_mutations:</t>
-  </si>
-  <si>
-    <t>authorizer</t>
-  </si>
-  <si>
-    <t>other:</t>
-  </si>
-  <si>
-    <t>helpers:</t>
-  </si>
-  <si>
-    <t>rating_satisfies_sheet</t>
-  </si>
-  <si>
-    <t>rating_sheet_of_category_id</t>
-  </si>
-  <si>
-    <t>global authorizer mw</t>
+    <t>commit transaction and end session</t>
   </si>
 </sst>
 </file>
@@ -695,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -717,6 +735,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3419,10 +3438,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B11F960-5BC5-40F2-A2DB-F955357F8F3E}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3430,9 +3449,10 @@
     <col min="1" max="1" width="16.77734375" customWidth="1"/>
     <col min="2" max="2" width="11.21875" customWidth="1"/>
     <col min="3" max="9" width="11.109375" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3456,7 +3476,7 @@
       <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -3497,23 +3517,23 @@
       <c r="G2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="21" t="s">
         <v>128</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>145</v>
+      <c r="K2" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="M2" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>145</v>
+      <c r="N2" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -3538,23 +3558,23 @@
       <c r="G3" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="22" t="s">
         <v>135</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>149</v>
+      <c r="K3" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>154</v>
+        <v>157</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -3574,28 +3594,28 @@
         <v>128</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="22" t="s">
         <v>135</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>150</v>
+      <c r="K4" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>144</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -3626,33 +3646,33 @@
       <c r="I5" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="N5" s="9" t="s">
+      <c r="K5" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M5" s="22" t="s">
         <v>147</v>
+      </c>
+      <c r="N5" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>147</v>
+      <c r="K6" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>169</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -3680,17 +3700,17 @@
       <c r="I7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>142</v>
+      <c r="K7" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>143</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>155</v>
+        <v>143</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -3718,17 +3738,17 @@
       <c r="I8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>159</v>
+      <c r="K8" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>178</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -3756,172 +3776,238 @@
       <c r="I9" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>86</v>
+      <c r="K9" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>172</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>144</v>
+        <v>170</v>
+      </c>
+      <c r="N9" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="N10" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="L11" s="22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K11" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="L11" s="2"/>
       <c r="M11" s="20" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>90</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L12" s="2"/>
+      <c r="K12" s="20" t="s">
+        <v>149</v>
+      </c>
       <c r="M12" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="N12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>158</v>
       </c>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C13" s="2"/>
-      <c r="D13" s="19" t="s">
-        <v>162</v>
+      <c r="C13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="I13" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="N13" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+        <v>152</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>140</v>
+      </c>
       <c r="M14" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="N14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M15" s="20" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>170</v>
-      </c>
-      <c r="B16" t="s">
-        <v>174</v>
-      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L16" s="9"/>
+      <c r="M16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>161</v>
+      </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H22" s="9"/>
+      <c r="K22">
+        <f>COUNTA(B2:I19)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H23" s="9"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H29" s="9"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PUT product half done
</commit_message>
<xml_diff>
--- a/trash/progress.xlsx
+++ b/trash/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\merged_sajt\trash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEFEB1F-51B4-4981-88AD-3E669C17C992}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D518E696-4534-4735-897E-CFF333466D60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" activeTab="2" xr2:uid="{012A0DE3-469E-4392-99CD-5887BA5AC192}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="184">
   <si>
     <t>Active_Password_Reset</t>
   </si>
@@ -575,6 +575,12 @@
   </si>
   <si>
     <t>find_in_tree</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>valid milk types</t>
   </si>
 </sst>
 </file>
@@ -3445,7 +3451,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3515,7 +3521,7 @@
       <c r="E2" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="18" t="s">
         <v>127</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -3530,10 +3536,10 @@
       <c r="K2" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="17" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="9" t="s">
@@ -3556,7 +3562,7 @@
       <c r="E3" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="19" t="s">
         <v>129</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -3571,10 +3577,10 @@
       <c r="K3" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="17" t="s">
         <v>157</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -3612,10 +3618,10 @@
       <c r="K4" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="17" t="s">
         <v>146</v>
       </c>
       <c r="N4" s="9" t="s">
@@ -3653,10 +3659,10 @@
       <c r="K5" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="19" t="s">
         <v>147</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -3666,13 +3672,13 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="17" t="s">
         <v>169</v>
       </c>
       <c r="N6" s="9" t="s">
@@ -3704,13 +3710,13 @@
       <c r="I7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="17" t="s">
         <v>143</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -3742,13 +3748,13 @@
       <c r="I8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="19" t="s">
         <v>175</v>
       </c>
       <c r="N8" s="9" t="s">
@@ -3780,13 +3786,13 @@
       <c r="I9" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="17" t="s">
         <v>170</v>
       </c>
       <c r="N9" s="2" t="s">
@@ -3818,13 +3824,13 @@
       <c r="I10" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="19" t="s">
         <v>171</v>
       </c>
       <c r="N10" s="2" t="s">
@@ -3856,10 +3862,10 @@
       <c r="I11" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="19" t="s">
         <v>86</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -3870,7 +3876,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="17" t="s">
         <v>149</v>
       </c>
       <c r="L12" s="2"/>
@@ -3902,7 +3908,7 @@
       <c r="I13" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="17" t="s">
         <v>172</v>
       </c>
       <c r="L13" s="2"/>
@@ -3927,7 +3933,7 @@
       <c r="I14" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="17" t="s">
         <v>140</v>
       </c>
       <c r="L14" s="2"/>
@@ -3948,7 +3954,7 @@
       <c r="I15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="17" t="s">
         <v>86</v>
       </c>
       <c r="L15" s="2"/>
@@ -4016,6 +4022,14 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H26" s="2"/>

</xml_diff>

<commit_message>
put user half done
</commit_message>
<xml_diff>
--- a/trash/progress.xlsx
+++ b/trash/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\merged_sajt\trash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF8FD16-31A5-4EC2-B15D-939869FDCFBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29239D54-8DD4-456C-8116-BFD8FB68E899}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" activeTab="2" xr2:uid="{012A0DE3-469E-4392-99CD-5887BA5AC192}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" tabRatio="512" activeTab="2" xr2:uid="{012A0DE3-469E-4392-99CD-5887BA5AC192}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -722,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -737,7 +737,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -747,6 +746,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3451,7 +3452,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3468,34 +3469,34 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="16" t="s">
         <v>98</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -3509,40 +3510,40 @@
       <c r="A2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>130</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>127</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="9" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3550,40 +3551,40 @@
       <c r="A3" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>131</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>129</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="2" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3591,37 +3592,37 @@
       <c r="A4" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>130</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>150</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>135</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="16" t="s">
         <v>146</v>
       </c>
       <c r="N4" s="9" t="s">
@@ -3632,37 +3633,37 @@
       <c r="A5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>128</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>130</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="19" t="s">
         <v>134</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="18" t="s">
         <v>147</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -3672,13 +3673,13 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="16" t="s">
         <v>169</v>
       </c>
       <c r="N6" s="9" t="s">
@@ -3710,13 +3711,13 @@
       <c r="I7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="16" t="s">
         <v>143</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -3748,13 +3749,13 @@
       <c r="I8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="9" t="s">
         <v>174</v>
       </c>
       <c r="N8" s="9" t="s">
@@ -3786,13 +3787,13 @@
       <c r="I9" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="2" t="s">
         <v>170</v>
       </c>
       <c r="N9" s="2" t="s">
@@ -3824,13 +3825,13 @@
       <c r="I10" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="9" t="s">
         <v>171</v>
       </c>
       <c r="N10" s="2" t="s">
@@ -3862,13 +3863,13 @@
       <c r="I11" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="2" t="s">
         <v>183</v>
       </c>
       <c r="N11" s="9" t="s">
@@ -3876,11 +3877,11 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="16" t="s">
         <v>149</v>
       </c>
       <c r="L12" s="2"/>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="2" t="s">
         <v>175</v>
       </c>
       <c r="N12" s="2" t="s">
@@ -3908,11 +3909,11 @@
       <c r="I13" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="16" t="s">
         <v>172</v>
       </c>
       <c r="L13" s="2"/>
-      <c r="M13" s="19" t="s">
+      <c r="M13" s="9" t="s">
         <v>149</v>
       </c>
       <c r="N13" s="9" t="s">
@@ -3921,7 +3922,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>152</v>
       </c>
       <c r="E14" s="2"/>
@@ -3933,11 +3934,11 @@
       <c r="I14" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="16" t="s">
         <v>140</v>
       </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="17" t="s">
+      <c r="M14" s="2" t="s">
         <v>176</v>
       </c>
       <c r="N14" s="9" t="s">
@@ -3954,11 +3955,11 @@
       <c r="I15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="16" t="s">
         <v>86</v>
       </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="17" t="s">
+      <c r="M15" s="2" t="s">
         <v>140</v>
       </c>
       <c r="N15" s="2"/>
@@ -3968,7 +3969,7 @@
       <c r="E16" s="9"/>
       <c r="K16" s="2"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="17" t="s">
+      <c r="M16" s="2" t="s">
         <v>86</v>
       </c>
       <c r="N16" s="9"/>

</xml_diff>

<commit_message>
now can begin frontend
</commit_message>
<xml_diff>
--- a/trash/progress.xlsx
+++ b/trash/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\merged_sajt\trash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7279226D-D4C2-45CE-ABB5-1EB8F9FFE480}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79473E4-2939-4B35-94FB-BADE259951A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" tabRatio="512" activeTab="4" xr2:uid="{012A0DE3-469E-4392-99CD-5887BA5AC192}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="204">
   <si>
     <t>Active_Password_Reset</t>
   </si>
@@ -617,18 +617,12 @@
     <t>router/api/mw/authorize.js</t>
   </si>
   <si>
-    <t>router/api/mw/check_authenticated.js</t>
-  </si>
-  <si>
     <t>router/api/mw/passport_authenticate.js</t>
   </si>
   <si>
     <t>router/api/mw/passport_initialize.js</t>
   </si>
   <si>
-    <t>router/api/mw/validate.js törlése, helyette validators/requests/api/akármi.js</t>
-  </si>
-  <si>
     <t>global error handling middleware</t>
   </si>
   <si>
@@ -644,7 +638,10 @@
     <t>joi validation of env variables</t>
   </si>
   <si>
-    <t>joi validator of api_request</t>
+    <t>router/api/mw/validate.js</t>
+  </si>
+  <si>
+    <t>all validators amik nem a modellek és a hozzájuk tartozó requestek</t>
   </si>
 </sst>
 </file>
@@ -792,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -807,7 +804,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -818,6 +814,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4570,10 +4568,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B11F960-5BC5-40F2-A2DB-F955357F8F3E}">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4590,37 +4588,37 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>99</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -4631,37 +4629,37 @@
       <c r="A2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>130</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>127</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="14" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="8" t="s">
@@ -4672,37 +4670,37 @@
       <c r="A3" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>128</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>131</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>129</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="14" t="s">
         <v>157</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -4713,37 +4711,37 @@
       <c r="A4" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>128</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>130</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>150</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="14" t="s">
         <v>146</v>
       </c>
       <c r="N4" s="8" t="s">
@@ -4754,37 +4752,37 @@
       <c r="A5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>128</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>130</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>134</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>130</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="16" t="s">
         <v>147</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -4794,13 +4792,13 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="14" t="s">
         <v>169</v>
       </c>
       <c r="N6" s="8" t="s">
@@ -4808,37 +4806,37 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="14" t="s">
         <v>143</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -4846,37 +4844,37 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M8" s="16" t="s">
         <v>174</v>
       </c>
       <c r="N8" s="8" t="s">
@@ -4884,37 +4882,37 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="14" t="s">
         <v>170</v>
       </c>
       <c r="N9" s="2" t="s">
@@ -4922,37 +4920,37 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="L10" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="16" t="s">
         <v>171</v>
       </c>
       <c r="N10" s="2" t="s">
@@ -4960,37 +4958,37 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="14" t="s">
         <v>182</v>
       </c>
       <c r="N11" s="8" t="s">
@@ -4998,11 +4996,11 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="14" t="s">
         <v>149</v>
       </c>
       <c r="L12" s="2"/>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="14" t="s">
         <v>175</v>
       </c>
       <c r="N12" s="2" t="s">
@@ -5013,28 +5011,28 @@
       <c r="A13" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="23" t="s">
         <v>151</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="23" t="s">
         <v>154</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="14" t="s">
         <v>172</v>
       </c>
       <c r="L13" s="2"/>
-      <c r="M13" s="17" t="s">
+      <c r="M13" s="16" t="s">
         <v>149</v>
       </c>
       <c r="N13" s="8" t="s">
@@ -5043,23 +5041,23 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="24" t="s">
         <v>152</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="23" t="s">
         <v>155</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>140</v>
       </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="14" t="s">
         <v>176</v>
       </c>
       <c r="N14" s="8" t="s">
@@ -5073,14 +5071,14 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="14" t="s">
         <v>86</v>
       </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="15" t="s">
+      <c r="M15" s="14" t="s">
         <v>140</v>
       </c>
       <c r="N15" s="2"/>
@@ -5090,7 +5088,7 @@
       <c r="E16" s="8"/>
       <c r="K16" s="2"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="15" t="s">
+      <c r="M16" s="14" t="s">
         <v>86</v>
       </c>
       <c r="N16" s="8"/>
@@ -5099,150 +5097,138 @@
       <c r="A17" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>164</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>183</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>184</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="B22" s="23" t="s">
         <v>193</v>
       </c>
       <c r="H22" s="8"/>
       <c r="K22">
         <f>COUNTA(B2:I100)</f>
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="B23" s="23" t="s">
         <v>190</v>
       </c>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="B24" s="23" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="B25" s="23" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="B26" s="23" t="s">
         <v>195</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+      <c r="B27" s="23" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>197</v>
+      <c r="B28" s="23" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>198</v>
+      <c r="B29" s="23" t="s">
+        <v>192</v>
       </c>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="B30" s="23" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>204</v>
+      <c r="A32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="23" t="s">
+        <v>163</v>
+      </c>
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>161</v>
-      </c>
-      <c r="B34" t="s">
-        <v>162</v>
+      <c r="B34" s="23" t="s">
+        <v>178</v>
       </c>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>163</v>
+      <c r="B35" s="23" t="s">
+        <v>179</v>
       </c>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>178</v>
-      </c>
-    </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>179</v>
+      <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>180</v>
-      </c>
-      <c r="B39" t="s">
-        <v>181</v>
+        <v>186</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="23" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>186</v>
-      </c>
-      <c r="B41" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+      <c r="B41" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5254,32 +5240,37 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16E4795-8244-4FA5-B14B-B51826EFF347}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>